<commit_message>
ExcelReport 2 : Hooks writeToExcel
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber_Kursu3\src\test\java\ApachePOI\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSM\IdeaProjects\Cucumber4\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AA43B3-7008-4A5D-8082-8C2A14D12904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="6000" yWindow="3540" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,58 +64,58 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulkemis11</t>
-  </si>
-  <si>
-    <t>ulkemis22</t>
-  </si>
-  <si>
-    <t>ulkemis33</t>
-  </si>
-  <si>
-    <t>ulkemis44</t>
-  </si>
-  <si>
-    <t>ulkemis55</t>
-  </si>
-  <si>
-    <t>ulkemis66</t>
-  </si>
-  <si>
-    <t>ulkemis77</t>
-  </si>
-  <si>
-    <t>ulkemis88</t>
-  </si>
-  <si>
-    <t>uis11</t>
-  </si>
-  <si>
-    <t>uis21</t>
-  </si>
-  <si>
-    <t>uis31</t>
-  </si>
-  <si>
-    <t>uis41</t>
-  </si>
-  <si>
-    <t>uis51</t>
-  </si>
-  <si>
-    <t>uis61</t>
-  </si>
-  <si>
-    <t>uis71</t>
-  </si>
-  <si>
-    <t>uis81</t>
+    <t>ulkemz22</t>
+  </si>
+  <si>
+    <t>ulkemz33</t>
+  </si>
+  <si>
+    <t>ulkemz44</t>
+  </si>
+  <si>
+    <t>ulkemz55</t>
+  </si>
+  <si>
+    <t>ulkemz66</t>
+  </si>
+  <si>
+    <t>ulkemz77</t>
+  </si>
+  <si>
+    <t>ulkemz88</t>
+  </si>
+  <si>
+    <t>ulkemz99</t>
+  </si>
+  <si>
+    <t>uz99</t>
+  </si>
+  <si>
+    <t>uz29</t>
+  </si>
+  <si>
+    <t>uz39</t>
+  </si>
+  <si>
+    <t>uz49</t>
+  </si>
+  <si>
+    <t>uz59</t>
+  </si>
+  <si>
+    <t>uz69</t>
+  </si>
+  <si>
+    <t>uz79</t>
+  </si>
+  <si>
+    <t>uz89</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,7 +427,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -509,11 +510,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +524,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -543,7 +544,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -563,7 +564,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -583,7 +584,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -603,7 +604,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
@@ -623,7 +624,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -643,7 +644,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -663,7 +664,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>

</xml_diff>